<commit_message>
docs: Agrega la estimación probable en la estimacion 5
</commit_message>
<xml_diff>
--- a/3. Etapa de construcción/Iteración 3/Estimacion/Estimación 5_Vesta Risk Manager_T-Code.xlsx
+++ b/3. Etapa de construcción/Iteración 3/Estimacion/Estimación 5_Vesta Risk Manager_T-Code.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Desktop\UNI\Analista de sistemas\Tercer año\Segundo cuatrimestre\Laboratorio de desarrollo de software\Git\develop\3. Etapa de construcción\Iteración 3\Estimacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAD1F84-F135-4CA8-8B0F-7E9C5636D490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2720B556-AB86-4155-98AF-FD3061063B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1927,7 +1927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
       <selection activeCell="B60" sqref="B60:F60"/>
     </sheetView>
   </sheetViews>
@@ -4115,11 +4115,11 @@
         <v>132</v>
       </c>
       <c r="F59" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G59" s="37">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -4152,7 +4152,7 @@
       <c r="F60" s="79"/>
       <c r="G60" s="17">
         <f>SUM(G52:G59)</f>
-        <v>26.5</v>
+        <v>28.5</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -4185,7 +4185,7 @@
       <c r="F61" s="79"/>
       <c r="G61" s="17">
         <f>1.4 + (-0.03*G60)</f>
-        <v>0.60499999999999998</v>
+        <v>0.54499999999999993</v>
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
@@ -4218,7 +4218,7 @@
       </c>
       <c r="G62" s="17">
         <f>COUNTIF($F$52:$F$57,"&lt;3")+COUNTIF($F$58:$F$59,"&gt;3")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -4309,7 +4309,7 @@
       <c r="F65" s="79"/>
       <c r="G65" s="46">
         <f>F30*G48*G61</f>
-        <v>56.87</v>
+        <v>51.22999999999999</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
@@ -4499,15 +4499,15 @@
       </c>
       <c r="B71" s="48">
         <f t="shared" ref="B71:D71" si="6">$G$65*B69</f>
-        <v>1137.3999999999999</v>
+        <v>1024.5999999999999</v>
       </c>
       <c r="C71" s="48">
         <f t="shared" si="6"/>
-        <v>1137.3999999999999</v>
+        <v>1024.5999999999999</v>
       </c>
       <c r="D71" s="48">
         <f t="shared" si="6"/>
-        <v>227.48</v>
+        <v>204.91999999999996</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="1"/>
@@ -4538,15 +4538,15 @@
       </c>
       <c r="B72" s="52">
         <f t="shared" ref="B72:D72" si="7">B71/(22*8)</f>
-        <v>6.4624999999999995</v>
+        <v>5.8215909090909088</v>
       </c>
       <c r="C72" s="52">
         <f t="shared" si="7"/>
-        <v>6.4624999999999995</v>
+        <v>5.8215909090909088</v>
       </c>
       <c r="D72" s="53">
         <f t="shared" si="7"/>
-        <v>1.2925</v>
+        <v>1.1643181818181816</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="1"/>
@@ -4707,15 +4707,15 @@
       </c>
       <c r="D77" s="52">
         <f t="shared" ref="D77:F77" si="8">$C77/$C$77*B$72</f>
-        <v>6.4624999999999995</v>
+        <v>5.8215909090909088</v>
       </c>
       <c r="E77" s="52">
         <f t="shared" si="8"/>
-        <v>6.4624999999999995</v>
+        <v>5.8215909090909088</v>
       </c>
       <c r="F77" s="52">
         <f t="shared" si="8"/>
-        <v>1.2925</v>
+        <v>1.1643181818181816</v>
       </c>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
@@ -4749,15 +4749,15 @@
       </c>
       <c r="D78" s="48">
         <f t="shared" ref="D78:F78" si="9">$C78/$C$77*B$72</f>
-        <v>9.6937499999999979</v>
+        <v>8.7323863636363619</v>
       </c>
       <c r="E78" s="48">
         <f t="shared" si="9"/>
-        <v>9.6937499999999979</v>
+        <v>8.7323863636363619</v>
       </c>
       <c r="F78" s="48">
         <f t="shared" si="9"/>
-        <v>1.9387499999999998</v>
+        <v>1.7464772727272722</v>
       </c>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
@@ -4789,15 +4789,15 @@
       </c>
       <c r="D79" s="52">
         <f t="shared" ref="D79:E79" si="10">$C79/$C$77*B$72</f>
-        <v>16.15625</v>
+        <v>14.553977272727272</v>
       </c>
       <c r="E79" s="52">
         <f t="shared" si="10"/>
-        <v>16.15625</v>
+        <v>14.553977272727272</v>
       </c>
       <c r="F79" s="52">
         <f>$C79/$C$77*D$72</f>
-        <v>3.2312500000000002</v>
+        <v>2.910795454545454</v>
       </c>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
@@ -4948,15 +4948,15 @@
       <c r="A84" s="60"/>
       <c r="B84" s="61">
         <f>$D$79/$B$81</f>
-        <v>5.385416666666667</v>
+        <v>4.8513257575757569</v>
       </c>
       <c r="C84" s="61">
         <f>$E$79/$B$81</f>
-        <v>5.385416666666667</v>
+        <v>4.8513257575757569</v>
       </c>
       <c r="D84" s="61">
         <f>$F$79/$B$81</f>
-        <v>1.0770833333333334</v>
+        <v>0.97026515151515136</v>
       </c>
       <c r="E84" s="60"/>
       <c r="F84" s="60"/>

</xml_diff>